<commit_message>
add local DB json
</commit_message>
<xml_diff>
--- a/client/src/assets/tracker/task tracker.xlsx
+++ b/client/src/assets/tracker/task tracker.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="85">
   <si>
     <t>Type</t>
   </si>
@@ -314,6 +314,9 @@
   </si>
   <si>
     <t>Activities  Data and websites images Collection ( Lanagar khana  etc  )</t>
+  </si>
+  <si>
+    <t>Local DB setup</t>
   </si>
 </sst>
 </file>
@@ -1051,8 +1054,8 @@
   </sheetPr>
   <dimension ref="B1:J64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1996,8 +1999,24 @@
       <c r="B39">
         <v>39</v>
       </c>
-      <c r="F39" s="3"/>
-      <c r="H39" s="3"/>
+      <c r="C39" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" s="3">
+        <v>45619</v>
+      </c>
+      <c r="G39" t="s">
+        <v>25</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="40" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B40">

</xml_diff>

<commit_message>
work on media page
</commit_message>
<xml_diff>
--- a/client/src/assets/tracker/task tracker.xlsx
+++ b/client/src/assets/tracker/task tracker.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" tabRatio="896" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5770" tabRatio="896" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Issue Tracker" sheetId="1" r:id="rId1"/>
@@ -773,7 +773,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -795,6 +795,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -853,7 +859,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -891,6 +897,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="10" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -1440,8 +1449,8 @@
   </sheetPr>
   <dimension ref="B1:J64"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView showGridLines="0" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2468,7 +2477,7 @@
       <c r="B45">
         <v>45</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="14" t="s">
         <v>96</v>
       </c>
       <c r="D45" t="s">
@@ -2492,7 +2501,7 @@
       <c r="B47">
         <v>47</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="14" t="s">
         <v>98</v>
       </c>
       <c r="D47" t="s">
@@ -5017,7 +5026,7 @@
         <v>*</v>
       </c>
     </row>
-    <row r="18" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="7:20" ht="77.5" x14ac:dyDescent="0.35">
       <c r="G18">
         <v>3</v>
       </c>
@@ -5083,7 +5092,7 @@
         <v>Medium</v>
       </c>
     </row>
-    <row r="20" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="7:20" ht="93" x14ac:dyDescent="0.35">
       <c r="G20">
         <v>5</v>
       </c>
@@ -5116,7 +5125,7 @@
         <v>Pakisatan</v>
       </c>
     </row>
-    <row r="21" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="7:20" ht="31" x14ac:dyDescent="0.35">
       <c r="G21">
         <v>6</v>
       </c>
@@ -5149,7 +5158,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="22" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="7:20" ht="139.5" x14ac:dyDescent="0.35">
       <c r="G22">
         <v>7</v>
       </c>
@@ -5182,7 +5191,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="23" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="7:20" ht="77.5" x14ac:dyDescent="0.35">
       <c r="G23">
         <v>8</v>
       </c>
@@ -6546,7 +6555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection sqref="A1:H63"/>
     </sheetView>
   </sheetViews>
@@ -7226,7 +7235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView topLeftCell="B55" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="A61" sqref="A2:H64"/>
     </sheetView>
   </sheetViews>
@@ -10137,7 +10146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -10736,7 +10745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
worked on book page
</commit_message>
<xml_diff>
--- a/client/src/assets/tracker/task tracker.xlsx
+++ b/client/src/assets/tracker/task tracker.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5770" tabRatio="896" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5770" tabRatio="896"/>
   </bookViews>
   <sheets>
     <sheet name="Issue Tracker" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="175">
   <si>
     <t>Type</t>
   </si>
@@ -607,6 +607,9 @@
   </si>
   <si>
     <t>BIO</t>
+  </si>
+  <si>
+    <t>media page isssue</t>
   </si>
 </sst>
 </file>
@@ -1196,8 +1199,8 @@
   </sheetPr>
   <dimension ref="B1:J64"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2230,6 +2233,9 @@
       <c r="D45" t="s">
         <v>84</v>
       </c>
+      <c r="E45" t="s">
+        <v>58</v>
+      </c>
       <c r="F45" s="3"/>
     </row>
     <row r="46" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -2242,6 +2248,9 @@
       <c r="D46" t="s">
         <v>85</v>
       </c>
+      <c r="E46" t="s">
+        <v>58</v>
+      </c>
       <c r="F46" s="3"/>
     </row>
     <row r="47" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -2254,11 +2263,20 @@
       <c r="D47" t="s">
         <v>86</v>
       </c>
+      <c r="E47" t="s">
+        <v>58</v>
+      </c>
       <c r="F47" s="3"/>
     </row>
     <row r="48" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B48">
         <v>48</v>
+      </c>
+      <c r="C48" t="s">
+        <v>174</v>
+      </c>
+      <c r="E48" t="s">
+        <v>58</v>
       </c>
       <c r="F48" s="3"/>
     </row>
@@ -2489,7 +2507,7 @@
       </c>
       <c r="O13">
         <f>COUNTA(O16:O45)-COUNTIF(O16:O45,NA())</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S13" t="s">
         <v>16</v>
@@ -2625,10 +2643,10 @@
       </c>
       <c r="T18" t="str">
         <f t="array" aca="1" ref="T18" ca="1">INDEX(prioritiesUnsorted, MATCH(SMALL(COUNTIF(prioritiesUnsorted, "&lt;"&amp;prioritiesUnsorted), ROW(3:3)), COUNTIF(prioritiesUnsorted, "&lt;"&amp;prioritiesUnsorted), 0))</f>
-        <v>High</v>
-      </c>
-    </row>
-    <row r="19" spans="7:20" ht="31" x14ac:dyDescent="0.35">
+        <v>done</v>
+      </c>
+    </row>
+    <row r="19" spans="7:20" x14ac:dyDescent="0.35">
       <c r="G19">
         <v>4</v>
       </c>
@@ -2658,7 +2676,7 @@
       </c>
       <c r="T19" t="str">
         <f t="array" aca="1" ref="T19" ca="1">INDEX(prioritiesUnsorted, MATCH(SMALL(COUNTIF(prioritiesUnsorted, "&lt;"&amp;prioritiesUnsorted), ROW(4:4)), COUNTIF(prioritiesUnsorted, "&lt;"&amp;prioritiesUnsorted), 0))</f>
-        <v>Medium</v>
+        <v>High</v>
       </c>
     </row>
     <row r="20" spans="7:20" ht="93" x14ac:dyDescent="0.35">
@@ -2681,9 +2699,9 @@
         <f t="array" ref="N20">INDEX(Issues[TYPE],MATCH(0,COUNTIF(N$15:N19, Issues[TYPE]),0))</f>
         <v>Add read books from website</v>
       </c>
-      <c r="O20" t="e">
+      <c r="O20" t="str">
         <f t="array" ref="O20">INDEX(Issues[PRIORITY],MATCH(0,COUNTIF(O$15:O19,Issues[PRIORITY]),0))</f>
-        <v>#N/A</v>
+        <v>done</v>
       </c>
       <c r="S20" t="str">
         <f t="array" aca="1" ref="S20" ca="1">INDEX(typesUnsorted, MATCH(SMALL(COUNTIF(typesUnsorted, "&lt;"&amp;typesUnsorted), ROW(5:5)), COUNTIF(typesUnsorted, "&lt;"&amp;typesUnsorted), 0))</f>
@@ -2691,7 +2709,7 @@
       </c>
       <c r="T20" t="str">
         <f t="array" aca="1" ref="T20" ca="1">INDEX(prioritiesUnsorted, MATCH(SMALL(COUNTIF(prioritiesUnsorted, "&lt;"&amp;prioritiesUnsorted), ROW(5:5)), COUNTIF(prioritiesUnsorted, "&lt;"&amp;prioritiesUnsorted), 0))</f>
-        <v>Pakisatan</v>
+        <v>Medium</v>
       </c>
     </row>
     <row r="21" spans="7:20" ht="31" x14ac:dyDescent="0.35">
@@ -2722,9 +2740,9 @@
         <f t="array" aca="1" ref="S21" ca="1">INDEX(typesUnsorted, MATCH(SMALL(COUNTIF(typesUnsorted, "&lt;"&amp;typesUnsorted), ROW(6:6)), COUNTIF(typesUnsorted, "&lt;"&amp;typesUnsorted), 0))</f>
         <v>Quran</v>
       </c>
-      <c r="T21" t="e">
+      <c r="T21" t="str">
         <f t="array" aca="1" ref="T21" ca="1">INDEX(prioritiesUnsorted, MATCH(SMALL(COUNTIF(prioritiesUnsorted, "&lt;"&amp;prioritiesUnsorted), ROW(6:6)), COUNTIF(prioritiesUnsorted, "&lt;"&amp;prioritiesUnsorted), 0))</f>
-        <v>#NUM!</v>
+        <v>Pakisatan</v>
       </c>
     </row>
     <row r="22" spans="7:20" ht="139.5" x14ac:dyDescent="0.35">
@@ -2760,7 +2778,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="23" spans="7:20" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="7:20" ht="62" x14ac:dyDescent="0.35">
       <c r="G23">
         <v>8</v>
       </c>
@@ -4830,7 +4848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>